<commit_message>
edited open crm to add pop up for logging in
</commit_message>
<xml_diff>
--- a/CRN and SBI Allocation/Config/Config.xlsx
+++ b/CRN and SBI Allocation/Config/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://defra-my.sharepoint.com/personal/marcey_winter_defra_gov_uk/Documents/UiPath - Working Folder/Racing Pigeon Loft Allocation Template/CRN and SBI Allocation/Config/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\x953923\Desktop\RPA-Racing-Pigeon-Loft-Allocation\CRN and SBI Allocation\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{ADDF25F2-BAC9-4B50-992F-4F4EA2A96A6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8CA7CEE-A3E4-42FB-AEB4-1CA023CF7714}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC45A071-5C01-4B6C-8AC2-C856DEE91A32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -182,30 +182,12 @@
     <t>RPLogInUrl</t>
   </si>
   <si>
-    <t>https://www-chs-perf.ruraldev.org.uk/login</t>
-  </si>
-  <si>
-    <t>Url to navigate to the Log In screen of the test version of RP</t>
-  </si>
-  <si>
     <t>RPHomeUrl</t>
   </si>
   <si>
-    <t>https://www-chs-perf.ruraldev.org.uk/#/internal_user/main</t>
-  </si>
-  <si>
-    <t>Url to navigate to the Home screenof the test version of RP</t>
-  </si>
-  <si>
     <t>RPCustomerUrl</t>
   </si>
   <si>
-    <t>https://www-chs-perf.ruraldev.org.uk/#/internal_user/dashboard/</t>
-  </si>
-  <si>
-    <t>Url to navigate to the customer details page of the test version of RP</t>
-  </si>
-  <si>
     <t>QueueName</t>
   </si>
   <si>
@@ -213,6 +195,33 @@
   </si>
   <si>
     <t>Queue name in CRM</t>
+  </si>
+  <si>
+    <t>Url to navigate to the customer details page of the live version of RP</t>
+  </si>
+  <si>
+    <t>Url to navigate to the Log In screen of the live version of RP</t>
+  </si>
+  <si>
+    <t>Url to navigate to the Home screenof the live version of RP</t>
+  </si>
+  <si>
+    <t>https://www.ruralpayments.service.gov.uk/login</t>
+  </si>
+  <si>
+    <t>https://www.ruralpayments.service.gov.uk/#/internal_user/main</t>
+  </si>
+  <si>
+    <t>https://www.ruralpayments.service.gov.uk/#/internal_user/dashboard/</t>
+  </si>
+  <si>
+    <t>PDFFilePath</t>
+  </si>
+  <si>
+    <t>C:\Users\{0}\Desktop\Working Directory\PDF.pdf</t>
+  </si>
+  <si>
+    <t>The full filepath to save the pdf document to</t>
   </si>
 </sst>
 </file>
@@ -280,7 +289,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -297,6 +306,10 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -616,7 +629,7 @@
   <dimension ref="A1:Z969"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="59.140625" defaultRowHeight="15" customHeight="1"/>
@@ -713,30 +726,95 @@
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" s="8"/>
+      <c r="C10" s="8"/>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" s="8"/>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A17" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -1686,7 +1764,7 @@
   <dimension ref="A1:Z987"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2799,7 +2877,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2844,61 +2922,11 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" t="s">
-        <v>49</v>
-      </c>
-    </row>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>